<commit_message>
descriptions visualisations, ajout conclusion, PDF rapport
</commit_message>
<xml_diff>
--- a/data/logs-tableau.xlsx
+++ b/data/logs-tableau.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethospatial/code/project/reveal.js/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE631AFA-5020-BA41-B8FC-06F18309124D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB141AE6-8DE5-A445-BCAA-B6C21D32B76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{13DC753A-4600-4E42-9C6B-49D759D11700}"/>
+    <workbookView xWindow="1460" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{13DC753A-4600-4E42-9C6B-49D759D11700}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="135">
   <si>
     <t xml:space="preserve"> Date     </t>
   </si>
@@ -386,6 +387,63 @@
   </si>
   <si>
     <t>Janvier</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Heure</t>
+  </si>
+  <si>
+    <t>Tâche</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Réaction du rapport </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction                   </t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Lecture et recherche de citations</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Intégration des citations de textes</t>
+  </si>
+  <si>
+    <t>Réorganisation du code, adaptation frise chronologique</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>RDV avec collègues, test</t>
+  </si>
+  <si>
+    <t>Tests / retours utilisateurices</t>
+  </si>
+  <si>
+    <t>Corrections du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction              </t>
+  </si>
+  <si>
+    <t>Fichier log.md revu et détaillés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction       </t>
+  </si>
+  <si>
+    <t>Intégration références prompts</t>
   </si>
 </sst>
 </file>
@@ -619,13 +677,13 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v> Tests / retours utilisateurices</c:v>
+                  <c:v> Traitement de données        </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v> Traitement de données        </c:v>
+                  <c:v> Réunion / coordination       </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v> Réunion / coordination       </c:v>
+                  <c:v> Tests / retours utilisateurices</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Conception</c:v>
@@ -652,22 +710,22 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,13 +1012,1010 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Tâches et temps consacrés au projet ISH</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil3!$C$10:$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v> Traitement de données        </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> Réunion / coordination       </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> Tests / retours utilisateurices</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Conception</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lecture / apprentissage</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rédaction</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Programmation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil3!$D$10:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-03DD-9345-964C-21949D839FD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="820643072"/>
+        <c:axId val="820644800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="820643072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Type de tâche</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820644800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="820644800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Heures consacrées</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820643072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1488,6 +2543,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4F20D6E-CF3B-D34D-9052-71299F2E53C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2192,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BB4D63-AFC6-9D45-A2D3-D095D56471AC}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="97" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A3" zoomScale="97" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3087,8 +4185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85B3B85-881F-AA44-8921-6C58AE1CDBCD}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -3107,6 +4205,9 @@
       <c r="B1" t="s">
         <v>50</v>
       </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
       <c r="K1" t="s">
         <v>110</v>
       </c>
@@ -3124,6 +4225,9 @@
       <c r="B2" t="s">
         <v>52</v>
       </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
       <c r="K2" t="s">
         <v>111</v>
       </c>
@@ -3141,6 +4245,9 @@
       <c r="B3" t="s">
         <v>52</v>
       </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
       <c r="K3" t="s">
         <v>111</v>
       </c>
@@ -3158,6 +4265,9 @@
       <c r="B4" t="s">
         <v>52</v>
       </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
       <c r="K4" t="s">
         <v>111</v>
       </c>
@@ -3175,6 +4285,9 @@
       <c r="B5" t="s">
         <v>52</v>
       </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
       <c r="K5" t="s">
         <v>111</v>
       </c>
@@ -3192,6 +4305,9 @@
       <c r="B6" t="s">
         <v>52</v>
       </c>
+      <c r="E6">
+        <v>31</v>
+      </c>
       <c r="K6" t="s">
         <v>111</v>
       </c>
@@ -3209,6 +4325,9 @@
       <c r="B7" t="s">
         <v>52</v>
       </c>
+      <c r="E7">
+        <v>75</v>
+      </c>
       <c r="K7" t="s">
         <v>111</v>
       </c>
@@ -3226,6 +4345,12 @@
       <c r="B8" t="s">
         <v>52</v>
       </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
       <c r="K8" t="s">
         <v>112</v>
       </c>
@@ -3242,12 +4367,6 @@
       </c>
       <c r="B9" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" t="s">
-        <v>109</v>
       </c>
       <c r="K9" t="s">
         <v>112</v>
@@ -3268,7 +4387,7 @@
         <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -3291,10 +4410,10 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K11" t="s">
         <v>112</v>
@@ -3314,10 +4433,10 @@
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K12" t="s">
         <v>112</v>
@@ -3363,7 +4482,7 @@
         <v>90</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K14" t="s">
         <v>112</v>
@@ -3386,7 +4505,7 @@
         <v>107</v>
       </c>
       <c r="D15">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s">
         <v>112</v>
@@ -3409,7 +4528,7 @@
         <v>96</v>
       </c>
       <c r="D16">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s">
         <v>112</v>
@@ -3444,6 +4563,10 @@
       </c>
       <c r="B18" t="s">
         <v>54</v>
+      </c>
+      <c r="D18">
+        <f>SUM(D10:D16)</f>
+        <v>193</v>
       </c>
       <c r="K18" t="s">
         <v>112</v>
@@ -4102,4 +5225,269 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF2B000-B1F8-8D45-B519-F8E2E486452E}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45827</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45828</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45830</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>